<commit_message>
Updated with exceptions and verifiers
</commit_message>
<xml_diff>
--- a/IJP-automation/src/test/resources/testdata/Data.xlsx
+++ b/IJP-automation/src/test/resources/testdata/Data.xlsx
@@ -1,40 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\IJP-automation\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{35D88823-4D5A-457D-986D-578176D24B92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15210" windowHeight="2175"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="20790" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProductDetails" sheetId="1" r:id="rId1"/>
     <sheet name="ReferenceData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
-  <si>
-    <t>Mobiles</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Number of Products</t>
   </si>
@@ -63,13 +51,13 @@
     <t>Sort dropdown</t>
   </si>
   <si>
-    <t>Purse</t>
+    <t>pens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -422,8 +410,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -438,35 +426,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
         <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -474,7 +451,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>ReferenceData!$A$2:$A$6</xm:f>
           </x14:formula1>
@@ -487,7 +464,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -501,32 +478,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>